<commit_message>
Removed report from repo
</commit_message>
<xml_diff>
--- a/DOE_model/factorial_params.xlsx
+++ b/DOE_model/factorial_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Werkmap\Obsidian\Github\RC-FAB-2D-Heterostructures\DOE_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F448D4-A856-4B08-8667-D32D408F3274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A91D4E3-4C5C-42AC-A9CA-68E66A5C3F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B11409B1-1748-4106-B2DF-C971854B53A2}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{B11409B1-1748-4106-B2DF-C971854B53A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -42,11 +42,21 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={7EE6BC95-7F54-422E-B8AE-F73FAC75196D}</author>
     <author>tc={89078540-DF50-418F-95F4-9756F20F8609}</author>
     <author>tc={F377E9B2-1295-487D-BB40-05CFC3303C19}</author>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{89078540-DF50-418F-95F4-9756F20F8609}">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{7EE6BC95-7F54-422E-B8AE-F73FAC75196D}">
+      <text>
+        <t xml:space="preserve">[Opmerkingenthread]
+U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
+Opmerking:
+    1 Hz
+</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{89078540-DF50-418F-95F4-9756F20F8609}">
       <text>
         <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -54,7 +64,7 @@
     Controlled by the tango desktop</t>
       </text>
     </comment>
-    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{F377E9B2-1295-487D-BB40-05CFC3303C19}">
+    <comment ref="B8" authorId="2" shapeId="0" xr:uid="{F377E9B2-1295-487D-BB40-05CFC3303C19}">
       <text>
         <t xml:space="preserve">[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -68,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>part name</t>
   </si>
@@ -76,12 +86,6 @@
     <t>step size (um)</t>
   </si>
   <si>
-    <t>min speed (um/s)</t>
-  </si>
-  <si>
-    <t>max speed (um/s)</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -164,13 +168,22 @@
   </si>
   <si>
     <t>Response (-)</t>
+  </si>
+  <si>
+    <t>min speed (steps/s)</t>
+  </si>
+  <si>
+    <t>max speed (steps/s)</t>
+  </si>
+  <si>
+    <t>Used acceleration (steps/s^2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +197,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -323,7 +342,7 @@
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>731520</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
@@ -400,7 +419,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>Elke meting duur 55 seconde (50 nodig om op top snelheid te komen en 5 sec speling. Voor elke meting word een achtergrond meting gedaan van dezefde tijd, dit is 'nodig' omdat de achtergrond vibratie in het lab over de dag varieerd</a:t>
+            <a:t>Elke meting duur 10 seconde (maximale tijd die gebruikt kan worden voor de onderdelen crashen)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -409,7 +428,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>All parts are tested using velosity control</a:t>
+            <a:t>All parts are tested using velosity control and the same acceleration. All parts start from their home position</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -725,6 +744,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E5" dT="2022-12-23T11:35:48.09" personId="{50D80062-D623-42FA-B49C-26D000ECE8E6}" id="{7EE6BC95-7F54-422E-B8AE-F73FAC75196D}">
+    <text xml:space="preserve">1 Hz
+</text>
+  </threadedComment>
   <threadedComment ref="B7" dT="2022-12-21T14:21:20.98" personId="{50D80062-D623-42FA-B49C-26D000ECE8E6}" id="{89078540-DF50-418F-95F4-9756F20F8609}">
     <text>Controlled by the tango desktop</text>
   </threadedComment>
@@ -737,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89A2BBB-2230-4309-927A-399AC88D1CD3}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,19 +773,20 @@
     <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.21875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -771,42 +795,45 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>0.02</v>
@@ -818,38 +845,39 @@
       <c r="E2" s="1">
         <v>40</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1"/>
+      <c r="G2" s="2">
         <v>0.5</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1">
-        <f t="shared" ref="J2:J5" si="0">E2/F2</f>
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2:K5" si="0">E2/G2</f>
         <v>80</v>
       </c>
-      <c r="K2" s="2">
-        <f>1/2 *F2*J2^2 /10000</f>
+      <c r="L2" s="2">
+        <f>1/2 *G2*K2^2 /10000</f>
         <v>0.16</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>1.4</v>
       </c>
-      <c r="M2" s="1">
-        <f>IF(K2&gt;L2, 0, 1)</f>
+      <c r="N2" s="1">
+        <f>IF(L2&gt;M2, 0, 1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>0.02</v>
@@ -861,38 +889,39 @@
       <c r="E3" s="1">
         <v>40</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1"/>
+      <c r="G3" s="2">
         <v>0.5</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="K3" s="2">
-        <f t="shared" ref="K3:K8" si="2">1/2 *F3*J3^2 /10000</f>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L8" si="2">1/2 *G3*K3^2 /10000</f>
         <v>0.16</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>1.4</v>
       </c>
-      <c r="M3" s="1">
-        <f t="shared" ref="M3:M8" si="3">IF(K3&gt;L3, 0, 1)</f>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N8" si="3">IF(L3&gt;M3, 0, 1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>0.02</v>
@@ -904,130 +933,139 @@
       <c r="E4" s="1">
         <v>40</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1"/>
+      <c r="G4" s="2">
         <v>0.5</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <f t="shared" si="2"/>
         <v>0.16</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>1.5</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>0.78125</v>
+        <f>0.78125 * 10</f>
+        <v>7.8125</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>-400</v>
+        <v>-25600</v>
       </c>
       <c r="E5" s="1">
-        <v>400</v>
-      </c>
-      <c r="F5" s="2">
-        <v>8</v>
-      </c>
-      <c r="G5" s="1">
-        <v>200</v>
+        <v>25600</v>
+      </c>
+      <c r="F5" s="1">
+        <v>600</v>
+      </c>
+      <c r="G5" s="2">
+        <f>E5/100</f>
+        <v>256</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
         <f>2.5*10^6 +5.5*10^6</f>
         <v>8000000</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="K5" s="2">
-        <f>1/2 *F5*J5^2 /10000</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
+        <v>100</v>
+      </c>
+      <c r="L5" s="2">
+        <f>1/2 *G5*C5*K5^2 /1000</f>
+        <v>10000</v>
+      </c>
+      <c r="M5" s="1">
         <v>8</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
-        <v>0.78125</v>
+        <v>7.81</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>-400</v>
+        <v>-25600</v>
       </c>
       <c r="E6" s="1">
-        <v>400</v>
-      </c>
-      <c r="F6" s="2">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1">
-        <v>200</v>
+        <v>25600</v>
+      </c>
+      <c r="F6" s="1">
+        <v>600</v>
+      </c>
+      <c r="G6" s="2">
+        <v>256</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
         <f>10*10^6</f>
         <v>10000000</v>
       </c>
-      <c r="J6" s="1">
-        <f>E6/F6</f>
-        <v>50</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="K6" s="1">
+        <f>E6/G6</f>
+        <v>100</v>
+      </c>
+      <c r="L6" s="2">
+        <f>1/2 *G6*C6*K6^2 /10000</f>
+        <v>999.68</v>
+      </c>
+      <c r="M6" s="1">
         <v>8</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
         <v>0.78125</v>
@@ -1039,41 +1077,42 @@
       <c r="E7" s="1">
         <v>7000</v>
       </c>
-      <c r="F7" s="2">
-        <f t="shared" ref="F7" si="4">10*C7</f>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2">
+        <f t="shared" ref="G7" si="4">10*C7</f>
         <v>7.8125</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>7000</v>
       </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
       <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
         <v>2000</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" ref="J7:J8" si="5">E7/F7</f>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7:K8" si="5">E7/G7</f>
         <v>896</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <f t="shared" si="2"/>
         <v>313.60000000000002</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>2.5</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>0.01</v>
@@ -1085,31 +1124,34 @@
       <c r="E8" s="1">
         <v>25</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2">
         <f>25/50</f>
         <v>0.5</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>25</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>-180</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>180</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>180</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -1126,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4DDB0A-9C54-4BA4-A51B-ACEF930E7ABE}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -1139,25 +1181,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>